<commit_message>
New reaction database format
</commit_message>
<xml_diff>
--- a/ecosysem/reactions/Excel/metabolisms.xlsx
+++ b/ecosysem/reactions/Excel/metabolisms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2424069M\Documents\GitHub\EcoSysEM\ecosysem\reactions\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emartinez\Documents\GitHub\EcoSysEM\ecosysem\reactions\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53ED16BA-8E63-4DF5-BB29-5FCEA365FB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A091556-EF43-41AC-906A-53AB8980891F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,12 +56,6 @@
     <t>H2O</t>
   </si>
   <si>
-    <t>CO/O2/CO2 (COOB)</t>
-  </si>
-  <si>
-    <t>H2/O2/H2O (HOB)</t>
-  </si>
-  <si>
     <t>H2</t>
   </si>
   <si>
@@ -74,9 +68,6 @@
     <t>S0</t>
   </si>
   <si>
-    <t>NH3/O2/NO2-/H2O/H+ (AOM)</t>
-  </si>
-  <si>
     <t>NH3</t>
   </si>
   <si>
@@ -86,19 +77,28 @@
     <t>NO3-</t>
   </si>
   <si>
-    <t>CH4/O2/CO2/H2O (Methanotrophs)</t>
-  </si>
-  <si>
     <t>CH4</t>
   </si>
   <si>
-    <t>H2S/O2/SO4-2/H+ (SOM)</t>
-  </si>
-  <si>
-    <t>H2S/O2/S0/H2O (HypSOM)</t>
-  </si>
-  <si>
-    <t>NH3/O2/NO3-/H2O/H+ (CMX)</t>
+    <t>Carbon monoxide oxidation (COOB)</t>
+  </si>
+  <si>
+    <t>Hydrogen oxidation (HOB)</t>
+  </si>
+  <si>
+    <t>Sulfur oxidation (SOM)</t>
+  </si>
+  <si>
+    <t>Hypoxic sulfur oxidation (HypSOM)</t>
+  </si>
+  <si>
+    <t>Ammonia oxidation (AOM)</t>
+  </si>
+  <si>
+    <t>Complete ammonia oxidation (CMX)</t>
+  </si>
+  <si>
+    <t>Methanotrophs (Mth)</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,30 +457,30 @@
     <col min="9" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -564,7 +564,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" s="4">
         <v>-2</v>
@@ -572,7 +572,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D8" s="4">
         <v>-1</v>
@@ -583,7 +583,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -591,7 +591,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E10" s="4">
         <v>1</v>
@@ -599,7 +599,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F11" s="4">
         <v>-1</v>
@@ -610,7 +610,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F12" s="4">
         <v>1</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G13" s="4">
         <v>1</v>
@@ -626,7 +626,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H14" s="4">
         <v>-1</v>

</xml_diff>